<commit_message>
second batch P08_6, creation P08_8 and revision P06_2, P13_3, P16_4, P25_1
</commit_message>
<xml_diff>
--- a/analysis/mails_01/P06_2/table_to_fill.xlsx
+++ b/analysis/mails_01/P06_2/table_to_fill.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">fieldsample_barcode</t>
   </si>
@@ -57,6 +57,162 @@
     <t xml:space="preserve">project_name</t>
   </si>
   <si>
+    <t xml:space="preserve">MFD13530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-10-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57.1088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polluted_soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langholt - Site B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subterranean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential pollution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subterranean – Polluted soil, city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langholt - Site B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13515</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langholt - Site B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13508</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFD13493</t>
+  </si>
+  <si>
     <t xml:space="preserve">MFD03235</t>
   </si>
   <si>
@@ -66,22 +222,16 @@
     <t xml:space="preserve">2019-11-07</t>
   </si>
   <si>
-    <t xml:space="preserve">57.0145</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.9854</t>
-  </si>
-  <si>
-    <t xml:space="preserve">polluted_soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subterranean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subterranean – Polluted soil, city</t>
+    <t xml:space="preserve">3120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freshwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater</t>
   </si>
   <si>
     <t xml:space="preserve">MFD03236</t>
@@ -163,17 +313,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBCE0A8"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -193,11 +338,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,24 +698,32 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2"/>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -588,24 +740,32 @@
       <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2"/>
       <c r="N3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -622,19 +782,1629 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" t="s">
+        <v>24</v>
+      </c>
+      <c r="L34" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" t="s">
+        <v>48</v>
+      </c>
+      <c r="I40" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" t="s">
+        <v>71</v>
+      </c>
+      <c r="L40" t="s">
+        <v>72</v>
+      </c>
+      <c r="M40" t="s">
+        <v>25</v>
+      </c>
+      <c r="N40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" t="s">
-        <v>22</v>
+      <c r="I41" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" t="s">
+        <v>71</v>
+      </c>
+      <c r="L41" t="s">
+        <v>72</v>
+      </c>
+      <c r="M41" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+      <c r="J42" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" t="s">
+        <v>71</v>
+      </c>
+      <c r="L42" t="s">
+        <v>72</v>
+      </c>
+      <c r="M42" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -653,10 +2423,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
@@ -664,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
@@ -672,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
@@ -680,7 +2450,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
@@ -688,7 +2458,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -696,7 +2466,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
@@ -704,7 +2474,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
@@ -712,7 +2482,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9">
@@ -720,7 +2490,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -728,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
@@ -736,7 +2506,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
@@ -744,7 +2514,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
@@ -752,7 +2522,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14">
@@ -760,7 +2530,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15">
@@ -768,7 +2538,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>